<commit_message>
Update Data and Dshboard xlsx file
</commit_message>
<xml_diff>
--- a/Task Management Tracker START (final dashboard).xlsx
+++ b/Task Management Tracker START (final dashboard).xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COUSERA\Excel project\Dynamic-Task-Management-Tracker-in-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25D5213-1D9F-4E5B-9B49-0940641D8014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE616870-14AA-4D94-84E6-686ADF607E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{1A5F5666-BE82-F64F-A80E-7F153D5D7E43}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{1A5F5666-BE82-F64F-A80E-7F153D5D7E43}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cover Page" sheetId="5" r:id="rId1"/>
-    <sheet name="Dashboard" sheetId="4" r:id="rId2"/>
-    <sheet name="Support Sheet" sheetId="2" r:id="rId3"/>
+    <sheet name="Dashboard" sheetId="4" r:id="rId1"/>
+    <sheet name="Support Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="age">#REF!</definedName>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t>Task Name</t>
   </si>
@@ -254,65 +253,6 @@
   </si>
   <si>
     <t>Team</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Get </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10% OFF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> our course using coupon code </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EMAIL10</t>
-    </r>
-  </si>
-  <si>
-    <t>Get our Excel for Business &amp; Finance Course</t>
-  </si>
-  <si>
-    <t>Go to Data Here</t>
-  </si>
-  <si>
-    <t>Made by Career Principles Ltd.</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>All content is copyright material of Career Principles Ltd.</t>
-  </si>
-  <si>
-    <t>This Excel model may not be reproduced or distributed by any means, including printing, 
-screencapturing, or any other method without the prior permission of the publisher.</t>
-  </si>
-  <si>
-    <t>Task Management Tracker</t>
   </si>
 </sst>
 </file>
@@ -322,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#&quot; Days&quot;"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -376,62 +316,6 @@
     </font>
     <font>
       <b/>
-      <sz val="60"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="20"/>
-      <color rgb="FF073673"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FF0432FF"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -439,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,18 +338,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF073673"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -473,110 +351,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,108 +373,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{D116B123-67C6-344C-8E97-773FA34E970D}"/>
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{D116B123-67C6-344C-8E97-773FA34E970D}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A1221B63-1151-9945-AD17-D34A8F7994D7}"/>
-    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{6371BA46-78D2-CF43-B416-26A12EFA2F80}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{6371BA46-78D2-CF43-B416-26A12EFA2F80}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -715,22 +416,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2580,51 +2268,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2487126</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>68813</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2648507" cy="921414"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A1658C-54A2-1D4C-934D-D1401417D79D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3960326" y="1465813"/>
-          <a:ext cx="2648507" cy="921414"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4246,7 +3889,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4348,20 +3991,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D19405D-7BA7-4D2F-B8D6-221757C255E1}" name="Table1" displayName="Table1" ref="B14:K29" totalsRowShown="0" headerRowDxfId="16" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D19405D-7BA7-4D2F-B8D6-221757C255E1}" name="Table1" displayName="Table1" ref="B14:K29" totalsRowShown="0" headerRowDxfId="10" headerRowCellStyle="Normal 2">
   <autoFilter ref="B14:K29" xr:uid="{4D19405D-7BA7-4D2F-B8D6-221757C255E1}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{53BA1ADF-9C71-4388-844A-523F7BC67C14}" name="Task ID" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{53BA1ADF-9C71-4388-844A-523F7BC67C14}" name="Task ID" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{48A967F0-94DA-4881-BC89-0BE8AF2BFEB0}" name="Task Name"/>
     <tableColumn id="3" xr3:uid="{390C247E-F8B0-453E-B39E-C2A5D19F2FE8}" name="Team"/>
     <tableColumn id="4" xr3:uid="{6B569940-8822-4BEE-B065-AD953F1C18F8}" name="Task Owner"/>
-    <tableColumn id="5" xr3:uid="{D1D96352-43E3-4626-8175-9495BF4D0013}" name="Start Date" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{9ECC08BE-9DA3-4762-B6E6-D10102E0E559}" name="Due Date" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{CDD30BFF-AD99-4B4F-98E0-01F6777C6B38}" name="Task Duration" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{D1D96352-43E3-4626-8175-9495BF4D0013}" name="Start Date" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{9ECC08BE-9DA3-4762-B6E6-D10102E0E559}" name="Due Date" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{CDD30BFF-AD99-4B4F-98E0-01F6777C6B38}" name="Task Duration" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{75C74665-4E21-404B-B8B2-3895ACFC871E}" name="Status" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{8A5D449E-699A-4198-872E-D43686B6ADFA}" name="Overdue?" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{75C74665-4E21-404B-B8B2-3895ACFC871E}" name="Status" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{8A5D449E-699A-4198-872E-D43686B6ADFA}" name="Overdue?" dataDxfId="4">
       <calculatedColumnFormula>AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{A84105D3-B029-4293-AF7F-42CB8A860F20}" name="Comments"/>
@@ -4686,132 +4329,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33356E0-76AA-174E-ACC1-F9D757CC725B}">
-  <dimension ref="B3:D18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="9"/>
-    <col min="2" max="2" width="8.5" style="9" customWidth="1"/>
-    <col min="3" max="3" width="95.6640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:4" ht="78" x14ac:dyDescent="0.4">
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="2:4" ht="11" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="10"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="2:4" ht="21" x14ac:dyDescent="0.5">
-      <c r="B7" s="10"/>
-      <c r="C7" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="2:4" ht="11" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="10"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:4" s="18" customFormat="1" ht="26" x14ac:dyDescent="0.4">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B10" s="10"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B11" s="10"/>
-      <c r="C11" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="10"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B13" s="10"/>
-      <c r="C13" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="10"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B15" s="10"/>
-      <c r="C15" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B16" s="10"/>
-      <c r="C16" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:4" ht="32" x14ac:dyDescent="0.4">
-      <c r="B17" s="10"/>
-      <c r="C17" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-    </row>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zwwAiLVQ4ObB2URpFUW07rgCsWZ6Uj8PRKvsewONocJsCSaKAooP+cvBYhXut+3VVqobFnklKRyrJcRByIKoKQ==" saltValue="XyrmH8SG+r5Rc89ogrCvpg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1" display="Get our VBA &amp; Macros Course" xr:uid="{094276ED-8C60-794A-802A-E39D1B6A24F2}"/>
-    <hyperlink ref="C11" location="Dashboard!A1" display="Go to Data Here" xr:uid="{B3D4263D-A5AD-B749-91D5-2DA9C1614126}"/>
-    <hyperlink ref="C13" r:id="rId2" display="Made by Kenji Explains" xr:uid="{754CA44A-D904-9543-B440-C8A3F3C59240}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28FA565C-E58D-E845-893A-5E7880C6E96F}">
   <dimension ref="B1:K29"/>
   <sheetViews>
@@ -4883,14 +4400,14 @@
       <c r="G15" s="2">
         <v>45920</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>18</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="28" t="b">
+      <c r="J15" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>0</v>
       </c>
@@ -4917,14 +4434,14 @@
       <c r="G16" s="2">
         <v>45925</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>20</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="28" t="b">
+      <c r="J16" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>0</v>
       </c>
@@ -4951,14 +4468,14 @@
       <c r="G17" s="2">
         <v>45874</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>26</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="28" t="b">
+      <c r="J17" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -4985,14 +4502,14 @@
       <c r="G18" s="2">
         <v>45930</v>
       </c>
-      <c r="H18" s="27">
+      <c r="H18" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>18</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="28" t="b">
+      <c r="J18" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>0</v>
       </c>
@@ -5019,14 +4536,14 @@
       <c r="G19" s="2">
         <v>45940</v>
       </c>
-      <c r="H19" s="27">
+      <c r="H19" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>25</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J19" s="28" t="b">
+      <c r="J19" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -5053,14 +4570,14 @@
       <c r="G20" s="2">
         <v>45945</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>27</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J20" s="28" t="b">
+      <c r="J20" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -5087,14 +4604,14 @@
       <c r="G21" s="2">
         <v>45896</v>
       </c>
-      <c r="H21" s="27">
+      <c r="H21" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>7</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="28" t="b">
+      <c r="J21" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -5121,14 +4638,14 @@
       <c r="G22" s="2">
         <v>45942</v>
       </c>
-      <c r="H22" s="27">
+      <c r="H22" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>20</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="28" t="b">
+      <c r="J22" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -5155,14 +4672,14 @@
       <c r="G23" s="2">
         <v>45950</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>27</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="28" t="b">
+      <c r="J23" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>0</v>
       </c>
@@ -5189,14 +4706,14 @@
       <c r="G24" s="2">
         <v>45935</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>11</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="28" t="b">
+      <c r="J24" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -5223,14 +4740,14 @@
       <c r="G25" s="2">
         <v>45932</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H25" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>7</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="28" t="b">
+      <c r="J25" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>0</v>
       </c>
@@ -5257,14 +4774,14 @@
       <c r="G26" s="2">
         <v>45960</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H26" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>34</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="28" t="b">
+      <c r="J26" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>0</v>
       </c>
@@ -5291,14 +4808,14 @@
       <c r="G27" s="2">
         <v>45937</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>10</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="28" t="b">
+      <c r="J27" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -5325,14 +4842,14 @@
       <c r="G28" s="2">
         <v>45948</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>20</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J28" s="28" t="b">
+      <c r="J28" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>0</v>
       </c>
@@ -5359,14 +4876,14 @@
       <c r="G29" s="2">
         <v>45934</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="7">
         <f>Table1[[#This Row],[Due Date]]-Table1[[#This Row],[Start Date]]</f>
         <v>5</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="28" t="b">
+      <c r="J29" s="8" t="b">
         <f ca="1">AND(Table1[[#This Row],[Status]]&lt;&gt;"Completed",Table1[[#This Row],[Due Date]]&lt;TODAY())</f>
         <v>1</v>
       </c>
@@ -5376,14 +4893,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I15:I29">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Completed"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"Not Started"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"Not Started"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J29">
@@ -5424,7 +4941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD76006-6B40-364D-90DA-E56E32DD5F29}">
   <dimension ref="B2:K10"/>
   <sheetViews>
@@ -5545,7 +5062,7 @@
       <c r="B6" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="6">
         <f>SUM(C3:C5)</f>
         <v>15</v>
       </c>

</xml_diff>